<commit_message>
el re fin LOKZ
</commit_message>
<xml_diff>
--- a/Docs/Modelo Físico/IndicesUsados.xlsx
+++ b/Docs/Modelo Físico/IndicesUsados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>ÍNDICE USADO</t>
   </si>
@@ -181,6 +181,120 @@
         <a:xfrm>
           <a:off x="762000" y="1857375"/>
           <a:ext cx="8534400" cy="1475849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8524875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38803</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762001" y="3533776"/>
+          <a:ext cx="8524874" cy="3553527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4962525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3057655</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="3419476"/>
+          <a:ext cx="4924425" cy="2981454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4743450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1466851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9701335</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5505450" y="3324226"/>
+          <a:ext cx="4957885" cy="3200400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,12 +606,12 @@
   <dimension ref="A1:D155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="128.7109375" customWidth="1"/>
+    <col min="2" max="2" width="146.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
@@ -538,21 +652,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="str">
+        <f>+C4</f>
+        <v>FECHAYHORA</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>+D4</f>
+        <v>Solo se requerira de los indices hechos por ORACLE yuno en FECHAYHORA( PEDIDO ) dado que solo se manejan llaves primarias y este atributo</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="276.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>

</xml_diff>